<commit_message>
Update with data from authors
</commit_message>
<xml_diff>
--- a/data/growth_data_Topt.xlsx
+++ b/data/growth_data_Topt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6424FB-6A89-C24F-B473-72F157DE9DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5638A226-AEAC-1146-ADF0-0E622E76FF25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12580" yWindow="460" windowWidth="21640" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="460" windowWidth="21640" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -357,9 +357,6 @@
     <t>Potentially average over a too large size-range; Geometric mean from size window; Unusual formula for SGR; Wild strain; Maturity size based on 16C treatment and 42% maturing (males); T_opt from fitted polynomial</t>
   </si>
   <si>
-    <t>Seawater treatment; Geometric mean from size window; Maturation size from Davis 1982 Aust. J. Mar. Freshwater Res</t>
-  </si>
-  <si>
     <t>Original unit in g/fish/day, converted by dividing by mass (g) and multiplying by 100; Optimum growth temperature = temperature at max growth</t>
   </si>
   <si>
@@ -369,9 +366,6 @@
     <t>Experiments not conducted at the same time (partly published previously); Maturation size 77.5 cm (Males 75, Females 80) (Icelandic cod at year 2000 Pardoe et al 2009 CJFAS); Temperature not from FishBase as it was not concistent with reference. Instead I used mean minimum and maximum from Righton et al (2010). Thermal niche of Atlantic cod Gadus morhua: limits, tolerance and optima. Marine Ecology Progress Series, 420, 1-13.</t>
   </si>
   <si>
-    <t>Growth is for a large size-range; Geometric mean average initial and final size</t>
-  </si>
-  <si>
     <t>Standard growth unit. different equation; Calculated sizes from mean TL using equation in Fig. 2; Multiple data points per temp and size, calculated mean in separate doc.; w_maturation from Craig et al 1981 CJFA, age at maturatity 2,3, used geometric mean of length at age.</t>
   </si>
   <si>
@@ -384,7 +378,13 @@
     <t>Zhang-etal-2016-JournalofAppliedIchtyology</t>
   </si>
   <si>
-    <t>Geometric mean from size window; Weight at maturation from midpoint in length in Foss et al 2004 Reviews in Fish Biology and Fisheries</t>
+    <t>Data from author (two measurements at warmest temp, took average); Geometric mean from size window; Weight at maturation from midpoint in length in Foss et al 2004 Reviews in Fish Biology and Fisheries</t>
+  </si>
+  <si>
+    <t>Data from author; Seawater treatment; Geometric mean from size window; Maturation size from Davis 1982 Aust. J. Mar. Freshwater Res</t>
+  </si>
+  <si>
+    <t>Growth is for a large size-range; Geometric mean average initial and final size; Data from author bud took from figure since not all data could be retrieved</t>
   </si>
 </sst>
 </file>
@@ -842,9 +842,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -877,7 +877,7 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>32</v>
@@ -1877,8 +1877,8 @@
       <c r="U15" s="15">
         <v>8.4</v>
       </c>
-      <c r="V15" s="14" t="s">
-        <v>110</v>
+      <c r="V15" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="W15" s="18" t="s">
         <v>31</v>
@@ -1942,8 +1942,8 @@
       <c r="U16" s="15">
         <v>8.4</v>
       </c>
-      <c r="V16" s="14" t="s">
-        <v>110</v>
+      <c r="V16" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="W16" s="18" t="s">
         <v>31</v>
@@ -2012,7 +2012,7 @@
         <v>27.05</v>
       </c>
       <c r="V17" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="W17" s="18" t="s">
         <v>96</v>
@@ -2081,7 +2081,7 @@
         <v>27.05</v>
       </c>
       <c r="V18" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="W18" s="18" t="s">
         <v>96</v>
@@ -2146,7 +2146,7 @@
         <v>5.4</v>
       </c>
       <c r="V19" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W19" s="18" t="s">
         <v>92</v>
@@ -2211,7 +2211,7 @@
         <v>5.4</v>
       </c>
       <c r="V20" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W20" s="18" t="s">
         <v>92</v>
@@ -2276,7 +2276,7 @@
         <v>5.4</v>
       </c>
       <c r="V21" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W21" s="18" t="s">
         <v>92</v>
@@ -2341,7 +2341,7 @@
         <v>5.4</v>
       </c>
       <c r="V22" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W22" s="18" t="s">
         <v>92</v>
@@ -2406,7 +2406,7 @@
         <v>5.4</v>
       </c>
       <c r="V23" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W23" s="18" t="s">
         <v>92</v>
@@ -2471,7 +2471,7 @@
         <v>5.4</v>
       </c>
       <c r="V24" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W24" s="18" t="s">
         <v>92</v>
@@ -2536,7 +2536,7 @@
         <v>5.4</v>
       </c>
       <c r="V25" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W25" s="18" t="s">
         <v>92</v>
@@ -2604,8 +2604,8 @@
       <c r="U26" s="15">
         <v>4.2</v>
       </c>
-      <c r="V26" s="14" t="s">
-        <v>114</v>
+      <c r="V26" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="W26" s="14" t="s">
         <v>36</v>
@@ -2673,8 +2673,8 @@
       <c r="U27" s="15">
         <v>4.2</v>
       </c>
-      <c r="V27" s="14" t="s">
-        <v>114</v>
+      <c r="V27" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="W27" s="14" t="s">
         <v>36</v>
@@ -2742,8 +2742,8 @@
       <c r="U28" s="15">
         <v>4.2</v>
       </c>
-      <c r="V28" s="14" t="s">
-        <v>114</v>
+      <c r="V28" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="W28" s="14" t="s">
         <v>36</v>
@@ -3198,7 +3198,7 @@
         <v>1.4</v>
       </c>
       <c r="V35" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="W35" s="14" t="s">
         <v>45</v>
@@ -3263,7 +3263,7 @@
         <v>1.4</v>
       </c>
       <c r="V36" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="W36" s="14" t="s">
         <v>45</v>
@@ -3328,7 +3328,7 @@
         <v>13.95</v>
       </c>
       <c r="V37" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W37" s="14" t="s">
         <v>48</v>
@@ -3393,7 +3393,7 @@
         <v>13.95</v>
       </c>
       <c r="V38" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W38" s="14" t="s">
         <v>48</v>
@@ -3458,7 +3458,7 @@
         <v>13.95</v>
       </c>
       <c r="V39" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W39" s="14" t="s">
         <v>48</v>
@@ -3523,7 +3523,7 @@
         <v>13.95</v>
       </c>
       <c r="V40" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W40" s="14" t="s">
         <v>48</v>
@@ -3588,10 +3588,10 @@
         <v>22</v>
       </c>
       <c r="V41" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="W41" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
@@ -3653,10 +3653,10 @@
         <v>22</v>
       </c>
       <c r="V42" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="W42" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
@@ -3718,10 +3718,10 @@
         <v>22</v>
       </c>
       <c r="V43" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="W43" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
@@ -3782,8 +3782,8 @@
       <c r="U44" s="15">
         <v>4.0999999999999996</v>
       </c>
-      <c r="V44" s="14" t="s">
-        <v>119</v>
+      <c r="V44" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="W44" s="14" t="s">
         <v>95</v>
@@ -3847,8 +3847,8 @@
       <c r="U45" s="15">
         <v>4.0999999999999996</v>
       </c>
-      <c r="V45" s="14" t="s">
-        <v>119</v>
+      <c r="V45" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="W45" s="14" t="s">
         <v>95</v>
@@ -3912,8 +3912,8 @@
       <c r="U46" s="15">
         <v>4.0999999999999996</v>
       </c>
-      <c r="V46" s="14" t="s">
-        <v>119</v>
+      <c r="V46" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="W46" s="14" t="s">
         <v>95</v>

</xml_diff>